<commit_message>
Update _Trans-files with the new regions + add transport possibility from MAR to DKW
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_ELC_ImportExport_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_ELC_ImportExport_Trans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SubRES_TMPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="210" documentId="13_ncr:1_{B8DD1E22-11D7-4741-9782-5216D9A55DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9319ACAA-B0F1-4995-A388-96C7953C63EA}"/>
+  <xr:revisionPtr revIDLastSave="212" documentId="13_ncr:1_{B8DD1E22-11D7-4741-9782-5216D9A55DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B93CB062-EA78-4927-BEB4-9E3B4F63757B}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="2790" windowWidth="16875" windowHeight="10523" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44880" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="25" r:id="rId1"/>
@@ -331,7 +331,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="291">
   <si>
     <t>DKE</t>
   </si>
@@ -1232,6 +1232,9 @@
   </si>
   <si>
     <t>EXPELC-DKISL3UK</t>
+  </si>
+  <si>
+    <t>MAR</t>
   </si>
 </sst>
 </file>
@@ -6969,81 +6972,6 @@
     <xf numFmtId="2" fontId="38" fillId="74" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="67" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="67" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="67" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="67" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="67" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="67" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="67" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="67" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="51" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="62" borderId="21" xfId="960" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="62" borderId="22" xfId="960" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="62" borderId="13" xfId="960" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="62" borderId="21" xfId="960" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="62" borderId="22" xfId="960" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="62" borderId="13" xfId="960" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="470" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="61" borderId="0" xfId="470" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -7053,6 +6981,81 @@
     <xf numFmtId="0" fontId="8" fillId="27" borderId="1" xfId="470" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="64" borderId="1" xfId="470" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="26" borderId="1" xfId="470" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="58" fillId="67" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="67" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="67" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="67" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="67" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="67" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="67" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="67" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="51" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="62" borderId="21" xfId="960" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="62" borderId="22" xfId="960" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="62" borderId="13" xfId="960" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="62" borderId="21" xfId="960" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="62" borderId="22" xfId="960" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="62" borderId="13" xfId="960" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2786">
     <cellStyle name="20 % - Akzent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -11422,10 +11425,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="C6:K32"/>
+  <dimension ref="C6:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="12.75"/>
@@ -11433,7 +11436,7 @@
     <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:11" ht="13.15">
+    <row r="6" spans="3:12" ht="13.15">
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
@@ -11442,7 +11445,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="3:11" ht="13.5" thickBot="1">
+    <row r="7" spans="3:12" ht="13.5" thickBot="1">
       <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
@@ -11470,8 +11473,11 @@
       <c r="K7" s="6" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="8" spans="3:11" ht="13.15">
+      <c r="L7" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" ht="13.15">
       <c r="C8" s="53"/>
       <c r="D8" s="50" t="s">
         <v>6</v>
@@ -11482,7 +11488,7 @@
       <c r="F8" s="52"/>
       <c r="G8" s="52"/>
     </row>
-    <row r="9" spans="3:11" ht="13.15">
+    <row r="9" spans="3:12" ht="13.15">
       <c r="C9" s="3"/>
       <c r="D9" s="67" t="s">
         <v>253</v>
@@ -11493,7 +11499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:11" ht="13.15">
+    <row r="10" spans="3:12" ht="13.15">
       <c r="C10" s="3"/>
       <c r="D10" s="47" t="s">
         <v>254</v>
@@ -11504,7 +11510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="3:11" ht="13.15">
+    <row r="11" spans="3:12" ht="13.15">
       <c r="C11" s="3"/>
       <c r="D11" s="46" t="s">
         <v>255</v>
@@ -11517,7 +11523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="3:11" ht="13.15">
+    <row r="12" spans="3:12" ht="13.15">
       <c r="C12" s="3"/>
       <c r="D12" s="46" t="s">
         <v>256</v>
@@ -11530,7 +11536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="3:11" ht="13.15">
+    <row r="13" spans="3:12" ht="13.15">
       <c r="C13" s="3"/>
       <c r="D13" s="67" t="s">
         <v>257</v>
@@ -11543,7 +11549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="3:11" ht="13.15">
+    <row r="14" spans="3:12" ht="13.15">
       <c r="C14" s="3"/>
       <c r="D14" s="47" t="s">
         <v>258</v>
@@ -11556,7 +11562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="3:11" ht="13.15">
+    <row r="15" spans="3:12" ht="13.15">
       <c r="C15" s="3"/>
       <c r="D15" s="46" t="s">
         <v>259</v>
@@ -11567,7 +11573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="3:11" ht="13.15">
+    <row r="16" spans="3:12" ht="13.15">
       <c r="C16" s="3"/>
       <c r="D16" s="46" t="s">
         <v>260</v>
@@ -11601,7 +11607,7 @@
       </c>
     </row>
     <row r="19" spans="3:11">
-      <c r="D19" s="429" t="s">
+      <c r="D19" s="404" t="s">
         <v>276</v>
       </c>
       <c r="H19">
@@ -11610,7 +11616,7 @@
     </row>
     <row r="20" spans="3:11">
       <c r="C20" s="43"/>
-      <c r="D20" s="429" t="s">
+      <c r="D20" s="404" t="s">
         <v>277</v>
       </c>
       <c r="H20">
@@ -11618,7 +11624,7 @@
       </c>
     </row>
     <row r="21" spans="3:11">
-      <c r="D21" s="429" t="s">
+      <c r="D21" s="404" t="s">
         <v>278</v>
       </c>
       <c r="I21">
@@ -11626,7 +11632,7 @@
       </c>
     </row>
     <row r="22" spans="3:11">
-      <c r="D22" s="429" t="s">
+      <c r="D22" s="404" t="s">
         <v>279</v>
       </c>
       <c r="J22">
@@ -11634,7 +11640,7 @@
       </c>
     </row>
     <row r="23" spans="3:11">
-      <c r="D23" s="429" t="s">
+      <c r="D23" s="404" t="s">
         <v>280</v>
       </c>
       <c r="K23">
@@ -11642,7 +11648,7 @@
       </c>
     </row>
     <row r="24" spans="3:11">
-      <c r="D24" s="429" t="s">
+      <c r="D24" s="404" t="s">
         <v>281</v>
       </c>
       <c r="I24">
@@ -11650,7 +11656,7 @@
       </c>
     </row>
     <row r="25" spans="3:11">
-      <c r="D25" s="429" t="s">
+      <c r="D25" s="404" t="s">
         <v>282</v>
       </c>
       <c r="J25">
@@ -11658,7 +11664,7 @@
       </c>
     </row>
     <row r="26" spans="3:11">
-      <c r="D26" s="429" t="s">
+      <c r="D26" s="404" t="s">
         <v>283</v>
       </c>
       <c r="K26">
@@ -11666,7 +11672,7 @@
       </c>
     </row>
     <row r="27" spans="3:11">
-      <c r="D27" s="429" t="s">
+      <c r="D27" s="404" t="s">
         <v>284</v>
       </c>
       <c r="I27">
@@ -11674,7 +11680,7 @@
       </c>
     </row>
     <row r="28" spans="3:11">
-      <c r="D28" s="429" t="s">
+      <c r="D28" s="404" t="s">
         <v>285</v>
       </c>
       <c r="J28">
@@ -11682,7 +11688,7 @@
       </c>
     </row>
     <row r="29" spans="3:11">
-      <c r="D29" s="429" t="s">
+      <c r="D29" s="404" t="s">
         <v>286</v>
       </c>
       <c r="K29">
@@ -11690,7 +11696,7 @@
       </c>
     </row>
     <row r="30" spans="3:11">
-      <c r="D30" s="429" t="s">
+      <c r="D30" s="404" t="s">
         <v>287</v>
       </c>
       <c r="I30">
@@ -11698,7 +11704,7 @@
       </c>
     </row>
     <row r="31" spans="3:11">
-      <c r="D31" s="429" t="s">
+      <c r="D31" s="404" t="s">
         <v>288</v>
       </c>
       <c r="J31">
@@ -11706,7 +11712,7 @@
       </c>
     </row>
     <row r="32" spans="3:11">
-      <c r="D32" s="429" t="s">
+      <c r="D32" s="404" t="s">
         <v>289</v>
       </c>
       <c r="K32">
@@ -11714,6 +11720,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="89" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
@@ -12094,53 +12101,53 @@
         <f>AVA!$D$13</f>
         <v>IMPELC-DKDE</v>
       </c>
-      <c r="M14" s="404" t="s">
+      <c r="M14" s="413" t="s">
         <v>16</v>
       </c>
-      <c r="N14" s="408">
+      <c r="N14" s="417">
         <v>2010</v>
       </c>
-      <c r="O14" s="409"/>
-      <c r="P14" s="410" t="s">
+      <c r="O14" s="418"/>
+      <c r="P14" s="419" t="s">
         <v>31</v>
       </c>
-      <c r="Q14" s="411"/>
-      <c r="R14" s="410">
+      <c r="Q14" s="420"/>
+      <c r="R14" s="419">
         <v>2015</v>
       </c>
-      <c r="S14" s="411"/>
-      <c r="T14" s="410">
+      <c r="S14" s="420"/>
+      <c r="T14" s="419">
         <v>2016</v>
       </c>
-      <c r="U14" s="411"/>
-      <c r="V14" s="410">
+      <c r="U14" s="420"/>
+      <c r="V14" s="419">
         <v>2017</v>
       </c>
-      <c r="W14" s="411"/>
-      <c r="X14" s="410">
+      <c r="W14" s="420"/>
+      <c r="X14" s="419">
         <v>2018</v>
       </c>
-      <c r="Y14" s="411"/>
-      <c r="Z14" s="410">
+      <c r="Y14" s="420"/>
+      <c r="Z14" s="419">
         <v>2019</v>
       </c>
-      <c r="AA14" s="411"/>
-      <c r="AB14" s="410">
+      <c r="AA14" s="420"/>
+      <c r="AB14" s="419">
         <v>2020</v>
       </c>
-      <c r="AC14" s="411"/>
-      <c r="AD14" s="406">
+      <c r="AC14" s="420"/>
+      <c r="AD14" s="415">
         <v>2025</v>
       </c>
-      <c r="AE14" s="407"/>
-      <c r="AF14" s="406">
+      <c r="AE14" s="416"/>
+      <c r="AF14" s="415">
         <v>2030</v>
       </c>
-      <c r="AG14" s="407"/>
-      <c r="AH14" s="406">
+      <c r="AG14" s="416"/>
+      <c r="AH14" s="415">
         <v>2035</v>
       </c>
-      <c r="AI14" s="407"/>
+      <c r="AI14" s="416"/>
       <c r="AL14"/>
       <c r="AM14"/>
       <c r="AN14"/>
@@ -12172,7 +12179,7 @@
         <f>AVA!$D$14</f>
         <v>EXPELC-DKDE</v>
       </c>
-      <c r="M15" s="405"/>
+      <c r="M15" s="414"/>
       <c r="N15" s="77" t="s">
         <v>14</v>
       </c>
@@ -16253,7 +16260,7 @@
   </sheetPr>
   <dimension ref="B4:AM129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+    <sheetView zoomScale="83" workbookViewId="0">
       <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
@@ -16400,40 +16407,40 @@
       <c r="M8" s="8"/>
     </row>
     <row r="9" spans="2:39" ht="13.15">
-      <c r="B9" s="434" t="s">
+      <c r="B9" s="409" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="434" t="s">
+      <c r="C9" s="409" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="434" t="s">
+      <c r="D9" s="409" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="434" t="s">
+      <c r="E9" s="409" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="435" t="s">
+      <c r="F9" s="410" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="435" t="s">
+      <c r="G9" s="410" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="435" t="s">
+      <c r="H9" s="410" t="s">
         <v>272</v>
       </c>
-      <c r="I9" s="435" t="s">
+      <c r="I9" s="410" t="s">
         <v>273</v>
       </c>
-      <c r="J9" s="435" t="s">
+      <c r="J9" s="410" t="s">
         <v>274</v>
       </c>
-      <c r="K9" s="435" t="s">
+      <c r="K9" s="410" t="s">
         <v>275</v>
       </c>
-      <c r="L9" s="436" t="s">
+      <c r="L9" s="411" t="s">
         <v>42</v>
       </c>
-      <c r="M9" s="437" t="s">
+      <c r="M9" s="412" t="s">
         <v>12</v>
       </c>
     </row>
@@ -16441,10 +16448,10 @@
       <c r="B10" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C10" s="430" t="s">
+      <c r="C10" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="431" t="s">
+      <c r="D10" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E10" s="28">
@@ -16475,10 +16482,10 @@
       <c r="B11" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C11" s="430" t="s">
+      <c r="C11" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="431" t="s">
+      <c r="D11" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E11" s="28">
@@ -16509,10 +16516,10 @@
       <c r="B12" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C12" s="430" t="s">
+      <c r="C12" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="431" t="s">
+      <c r="D12" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E12" s="28">
@@ -16546,10 +16553,10 @@
       <c r="B13" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C13" s="430" t="s">
+      <c r="C13" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="431" t="s">
+      <c r="D13" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E13" s="28">
@@ -16583,10 +16590,10 @@
       <c r="B14" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C14" s="430" t="s">
+      <c r="C14" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="431" t="s">
+      <c r="D14" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E14" s="28">
@@ -16620,10 +16627,10 @@
       <c r="B15" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C15" s="430" t="s">
+      <c r="C15" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="431" t="s">
+      <c r="D15" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E15" s="28">
@@ -16657,10 +16664,10 @@
       <c r="B16" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C16" s="430" t="s">
+      <c r="C16" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="431" t="s">
+      <c r="D16" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E16" s="28">
@@ -16675,7 +16682,7 @@
       <c r="L16" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M16" s="433" t="s">
+      <c r="M16" s="408" t="s">
         <v>276</v>
       </c>
       <c r="AJ16"/>
@@ -16687,10 +16694,10 @@
       <c r="B17" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C17" s="430" t="s">
+      <c r="C17" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="431" t="s">
+      <c r="D17" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E17" s="28">
@@ -16705,7 +16712,7 @@
       <c r="L17" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M17" s="433" t="s">
+      <c r="M17" s="408" t="s">
         <v>277</v>
       </c>
       <c r="AJ17"/>
@@ -16717,10 +16724,10 @@
       <c r="B18" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C18" s="430" t="s">
+      <c r="C18" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="431" t="s">
+      <c r="D18" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E18" s="28">
@@ -16735,7 +16742,7 @@
       <c r="L18" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M18" s="433" t="s">
+      <c r="M18" s="408" t="s">
         <v>278</v>
       </c>
       <c r="AJ18"/>
@@ -16747,10 +16754,10 @@
       <c r="B19" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C19" s="430" t="s">
+      <c r="C19" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="431" t="s">
+      <c r="D19" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E19" s="28">
@@ -16765,7 +16772,7 @@
       <c r="L19" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M19" s="433" t="s">
+      <c r="M19" s="408" t="s">
         <v>279</v>
       </c>
       <c r="AJ19"/>
@@ -16777,10 +16784,10 @@
       <c r="B20" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C20" s="430" t="s">
+      <c r="C20" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="431" t="s">
+      <c r="D20" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E20" s="28">
@@ -16795,7 +16802,7 @@
       <c r="L20" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M20" s="433" t="s">
+      <c r="M20" s="408" t="s">
         <v>280</v>
       </c>
       <c r="AJ20"/>
@@ -16807,10 +16814,10 @@
       <c r="B21" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C21" s="430" t="s">
+      <c r="C21" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="431" t="s">
+      <c r="D21" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E21" s="28">
@@ -16825,7 +16832,7 @@
       <c r="L21" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M21" s="433" t="s">
+      <c r="M21" s="408" t="s">
         <v>281</v>
       </c>
       <c r="AJ21"/>
@@ -16837,10 +16844,10 @@
       <c r="B22" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C22" s="430" t="s">
+      <c r="C22" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="431" t="s">
+      <c r="D22" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E22" s="28">
@@ -16855,7 +16862,7 @@
       <c r="L22" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M22" s="433" t="s">
+      <c r="M22" s="408" t="s">
         <v>282</v>
       </c>
       <c r="AJ22"/>
@@ -16867,10 +16874,10 @@
       <c r="B23" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C23" s="430" t="s">
+      <c r="C23" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="431" t="s">
+      <c r="D23" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E23" s="28">
@@ -16885,7 +16892,7 @@
       <c r="L23" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M23" s="433" t="s">
+      <c r="M23" s="408" t="s">
         <v>283</v>
       </c>
       <c r="AJ23"/>
@@ -16897,10 +16904,10 @@
       <c r="B24" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C24" s="430" t="s">
+      <c r="C24" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="431" t="s">
+      <c r="D24" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E24" s="28">
@@ -16915,7 +16922,7 @@
       <c r="L24" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M24" s="433" t="s">
+      <c r="M24" s="408" t="s">
         <v>284</v>
       </c>
       <c r="AJ24"/>
@@ -16927,10 +16934,10 @@
       <c r="B25" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C25" s="430" t="s">
+      <c r="C25" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="431" t="s">
+      <c r="D25" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E25" s="28">
@@ -16945,7 +16952,7 @@
       <c r="L25" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M25" s="433" t="s">
+      <c r="M25" s="408" t="s">
         <v>285</v>
       </c>
       <c r="AJ25"/>
@@ -16957,10 +16964,10 @@
       <c r="B26" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C26" s="430" t="s">
+      <c r="C26" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="431" t="s">
+      <c r="D26" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E26" s="28">
@@ -16975,7 +16982,7 @@
       <c r="L26" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M26" s="433" t="s">
+      <c r="M26" s="408" t="s">
         <v>286</v>
       </c>
       <c r="AJ26"/>
@@ -16987,10 +16994,10 @@
       <c r="B27" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="430" t="s">
+      <c r="C27" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="431" t="s">
+      <c r="D27" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E27" s="28">
@@ -17005,7 +17012,7 @@
       <c r="L27" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M27" s="433" t="s">
+      <c r="M27" s="408" t="s">
         <v>287</v>
       </c>
       <c r="AJ27"/>
@@ -17017,10 +17024,10 @@
       <c r="B28" s="398" t="s">
         <v>175</v>
       </c>
-      <c r="C28" s="430" t="s">
+      <c r="C28" s="405" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="431" t="s">
+      <c r="D28" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E28" s="28">
@@ -17035,7 +17042,7 @@
       <c r="L28" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M28" s="433" t="s">
+      <c r="M28" s="408" t="s">
         <v>288</v>
       </c>
       <c r="AJ28"/>
@@ -17065,7 +17072,7 @@
       <c r="L29" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="M29" s="432" t="s">
+      <c r="M29" s="407" t="s">
         <v>289</v>
       </c>
       <c r="AJ29"/>
@@ -17080,7 +17087,7 @@
       <c r="C30" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="431" t="s">
+      <c r="D30" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E30" s="29">
@@ -17114,7 +17121,7 @@
       <c r="C31" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="431" t="s">
+      <c r="D31" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E31" s="29">
@@ -17148,7 +17155,7 @@
       <c r="C32" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="431" t="s">
+      <c r="D32" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E32" s="29">
@@ -17185,7 +17192,7 @@
       <c r="C33" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="431" t="s">
+      <c r="D33" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E33" s="29">
@@ -17222,7 +17229,7 @@
       <c r="C34" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="431" t="s">
+      <c r="D34" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E34" s="29">
@@ -17259,7 +17266,7 @@
       <c r="C35" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="431" t="s">
+      <c r="D35" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E35" s="29">
@@ -17296,7 +17303,7 @@
       <c r="C36" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="431" t="s">
+      <c r="D36" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E36" s="29">
@@ -17311,7 +17318,7 @@
       <c r="L36" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M36" s="433" t="s">
+      <c r="M36" s="408" t="s">
         <v>276</v>
       </c>
       <c r="AJ36"/>
@@ -17326,7 +17333,7 @@
       <c r="C37" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="431" t="s">
+      <c r="D37" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E37" s="29">
@@ -17341,7 +17348,7 @@
       <c r="L37" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M37" s="433" t="s">
+      <c r="M37" s="408" t="s">
         <v>277</v>
       </c>
       <c r="AJ37"/>
@@ -17356,7 +17363,7 @@
       <c r="C38" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="431" t="s">
+      <c r="D38" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E38" s="29">
@@ -17371,7 +17378,7 @@
       <c r="L38" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M38" s="433" t="s">
+      <c r="M38" s="408" t="s">
         <v>278</v>
       </c>
       <c r="AJ38"/>
@@ -17386,7 +17393,7 @@
       <c r="C39" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="431" t="s">
+      <c r="D39" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E39" s="29">
@@ -17401,7 +17408,7 @@
       <c r="L39" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M39" s="433" t="s">
+      <c r="M39" s="408" t="s">
         <v>279</v>
       </c>
       <c r="AJ39"/>
@@ -17416,7 +17423,7 @@
       <c r="C40" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="431" t="s">
+      <c r="D40" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E40" s="29">
@@ -17431,7 +17438,7 @@
       <c r="L40" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M40" s="433" t="s">
+      <c r="M40" s="408" t="s">
         <v>280</v>
       </c>
       <c r="AJ40"/>
@@ -17446,7 +17453,7 @@
       <c r="C41" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="431" t="s">
+      <c r="D41" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E41" s="29">
@@ -17461,7 +17468,7 @@
       <c r="L41" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M41" s="433" t="s">
+      <c r="M41" s="408" t="s">
         <v>281</v>
       </c>
       <c r="AJ41"/>
@@ -17476,7 +17483,7 @@
       <c r="C42" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="431" t="s">
+      <c r="D42" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E42" s="29">
@@ -17491,7 +17498,7 @@
       <c r="L42" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M42" s="433" t="s">
+      <c r="M42" s="408" t="s">
         <v>282</v>
       </c>
       <c r="AJ42"/>
@@ -17506,7 +17513,7 @@
       <c r="C43" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="431" t="s">
+      <c r="D43" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E43" s="29">
@@ -17521,7 +17528,7 @@
       <c r="L43" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M43" s="433" t="s">
+      <c r="M43" s="408" t="s">
         <v>283</v>
       </c>
       <c r="AJ43"/>
@@ -17536,7 +17543,7 @@
       <c r="C44" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D44" s="431" t="s">
+      <c r="D44" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E44" s="29">
@@ -17551,7 +17558,7 @@
       <c r="L44" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M44" s="433" t="s">
+      <c r="M44" s="408" t="s">
         <v>284</v>
       </c>
       <c r="AJ44"/>
@@ -17566,7 +17573,7 @@
       <c r="C45" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D45" s="431" t="s">
+      <c r="D45" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E45" s="29">
@@ -17581,7 +17588,7 @@
       <c r="L45" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M45" s="433" t="s">
+      <c r="M45" s="408" t="s">
         <v>285</v>
       </c>
       <c r="AJ45"/>
@@ -17596,7 +17603,7 @@
       <c r="C46" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D46" s="431" t="s">
+      <c r="D46" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E46" s="29">
@@ -17611,7 +17618,7 @@
       <c r="L46" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M46" s="433" t="s">
+      <c r="M46" s="408" t="s">
         <v>286</v>
       </c>
       <c r="AJ46"/>
@@ -17626,7 +17633,7 @@
       <c r="C47" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="431" t="s">
+      <c r="D47" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E47" s="29">
@@ -17641,7 +17648,7 @@
       <c r="L47" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M47" s="433" t="s">
+      <c r="M47" s="408" t="s">
         <v>287</v>
       </c>
       <c r="AJ47"/>
@@ -17656,7 +17663,7 @@
       <c r="C48" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D48" s="431" t="s">
+      <c r="D48" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E48" s="29">
@@ -17671,7 +17678,7 @@
       <c r="L48" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M48" s="433" t="s">
+      <c r="M48" s="408" t="s">
         <v>288</v>
       </c>
       <c r="AJ48"/>
@@ -17701,7 +17708,7 @@
       <c r="L49" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="M49" s="432" t="s">
+      <c r="M49" s="407" t="s">
         <v>289</v>
       </c>
       <c r="AJ49"/>
@@ -17716,7 +17723,7 @@
       <c r="C50" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D50" s="431" t="s">
+      <c r="D50" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E50" s="32">
@@ -17750,7 +17757,7 @@
       <c r="C51" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D51" s="431" t="s">
+      <c r="D51" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E51" s="29">
@@ -17784,7 +17791,7 @@
       <c r="C52" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D52" s="431" t="s">
+      <c r="D52" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E52" s="29">
@@ -17823,7 +17830,7 @@
       <c r="C53" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D53" s="431" t="s">
+      <c r="D53" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E53" s="29">
@@ -17864,7 +17871,7 @@
       <c r="C54" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D54" s="431" t="s">
+      <c r="D54" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E54" s="29">
@@ -17899,7 +17906,7 @@
       <c r="C55" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D55" s="431" t="s">
+      <c r="D55" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E55" s="29">
@@ -17935,7 +17942,7 @@
       <c r="C56" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D56" s="431" t="s">
+      <c r="D56" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E56" s="29">
@@ -17950,7 +17957,7 @@
       <c r="L56" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M56" s="433" t="s">
+      <c r="M56" s="408" t="s">
         <v>276</v>
       </c>
       <c r="N56" s="26"/>
@@ -17964,7 +17971,7 @@
       <c r="C57" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D57" s="431" t="s">
+      <c r="D57" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E57" s="29">
@@ -17979,7 +17986,7 @@
       <c r="L57" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M57" s="433" t="s">
+      <c r="M57" s="408" t="s">
         <v>277</v>
       </c>
       <c r="N57" s="26"/>
@@ -17993,7 +18000,7 @@
       <c r="C58" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D58" s="431" t="s">
+      <c r="D58" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E58" s="29">
@@ -18008,7 +18015,7 @@
       <c r="L58" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M58" s="433" t="s">
+      <c r="M58" s="408" t="s">
         <v>278</v>
       </c>
       <c r="N58" s="26"/>
@@ -18022,7 +18029,7 @@
       <c r="C59" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D59" s="431" t="s">
+      <c r="D59" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E59" s="29">
@@ -18037,7 +18044,7 @@
       <c r="L59" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M59" s="433" t="s">
+      <c r="M59" s="408" t="s">
         <v>279</v>
       </c>
       <c r="N59" s="26"/>
@@ -18051,7 +18058,7 @@
       <c r="C60" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D60" s="431" t="s">
+      <c r="D60" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E60" s="29">
@@ -18066,7 +18073,7 @@
       <c r="L60" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M60" s="433" t="s">
+      <c r="M60" s="408" t="s">
         <v>280</v>
       </c>
       <c r="N60" s="26"/>
@@ -18080,7 +18087,7 @@
       <c r="C61" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D61" s="431" t="s">
+      <c r="D61" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E61" s="29">
@@ -18095,7 +18102,7 @@
       <c r="L61" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M61" s="433" t="s">
+      <c r="M61" s="408" t="s">
         <v>281</v>
       </c>
       <c r="N61" s="26"/>
@@ -18109,7 +18116,7 @@
       <c r="C62" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D62" s="431" t="s">
+      <c r="D62" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E62" s="29">
@@ -18124,7 +18131,7 @@
       <c r="L62" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M62" s="433" t="s">
+      <c r="M62" s="408" t="s">
         <v>282</v>
       </c>
       <c r="N62" s="26"/>
@@ -18138,7 +18145,7 @@
       <c r="C63" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D63" s="431" t="s">
+      <c r="D63" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E63" s="29">
@@ -18153,7 +18160,7 @@
       <c r="L63" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M63" s="433" t="s">
+      <c r="M63" s="408" t="s">
         <v>283</v>
       </c>
       <c r="N63" s="26"/>
@@ -18167,7 +18174,7 @@
       <c r="C64" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D64" s="431" t="s">
+      <c r="D64" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E64" s="29">
@@ -18182,7 +18189,7 @@
       <c r="L64" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M64" s="433" t="s">
+      <c r="M64" s="408" t="s">
         <v>284</v>
       </c>
       <c r="N64" s="26"/>
@@ -18196,7 +18203,7 @@
       <c r="C65" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D65" s="431" t="s">
+      <c r="D65" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E65" s="29">
@@ -18211,7 +18218,7 @@
       <c r="L65" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M65" s="433" t="s">
+      <c r="M65" s="408" t="s">
         <v>285</v>
       </c>
       <c r="N65" s="26"/>
@@ -18225,7 +18232,7 @@
       <c r="C66" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D66" s="431" t="s">
+      <c r="D66" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E66" s="29">
@@ -18240,7 +18247,7 @@
       <c r="L66" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M66" s="433" t="s">
+      <c r="M66" s="408" t="s">
         <v>286</v>
       </c>
       <c r="N66" s="26"/>
@@ -18254,7 +18261,7 @@
       <c r="C67" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D67" s="431" t="s">
+      <c r="D67" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E67" s="29">
@@ -18269,7 +18276,7 @@
       <c r="L67" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M67" s="433" t="s">
+      <c r="M67" s="408" t="s">
         <v>287</v>
       </c>
       <c r="N67" s="26"/>
@@ -18283,7 +18290,7 @@
       <c r="C68" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D68" s="431" t="s">
+      <c r="D68" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E68" s="29">
@@ -18298,7 +18305,7 @@
       <c r="L68" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M68" s="433" t="s">
+      <c r="M68" s="408" t="s">
         <v>288</v>
       </c>
       <c r="N68" s="26"/>
@@ -18327,7 +18334,7 @@
       <c r="L69" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="M69" s="432" t="s">
+      <c r="M69" s="407" t="s">
         <v>289</v>
       </c>
       <c r="N69" s="26"/>
@@ -18341,7 +18348,7 @@
       <c r="C70" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D70" s="431" t="s">
+      <c r="D70" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E70" s="29">
@@ -18371,7 +18378,7 @@
       <c r="C71" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D71" s="431" t="s">
+      <c r="D71" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E71" s="29">
@@ -18401,7 +18408,7 @@
       <c r="C72" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D72" s="431" t="s">
+      <c r="D72" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E72" s="29">
@@ -18434,7 +18441,7 @@
       <c r="C73" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D73" s="431" t="s">
+      <c r="D73" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E73" s="29">
@@ -18467,7 +18474,7 @@
       <c r="C74" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D74" s="431" t="s">
+      <c r="D74" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E74" s="29">
@@ -18501,7 +18508,7 @@
       <c r="C75" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D75" s="431" t="s">
+      <c r="D75" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E75" s="29">
@@ -18534,7 +18541,7 @@
       <c r="C76" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D76" s="431" t="s">
+      <c r="D76" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E76" s="29">
@@ -18549,7 +18556,7 @@
       <c r="L76" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M76" s="433" t="s">
+      <c r="M76" s="408" t="s">
         <v>276</v>
       </c>
     </row>
@@ -18560,7 +18567,7 @@
       <c r="C77" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D77" s="431" t="s">
+      <c r="D77" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E77" s="29">
@@ -18575,7 +18582,7 @@
       <c r="L77" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M77" s="433" t="s">
+      <c r="M77" s="408" t="s">
         <v>277</v>
       </c>
     </row>
@@ -18586,7 +18593,7 @@
       <c r="C78" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D78" s="431" t="s">
+      <c r="D78" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E78" s="29">
@@ -18601,7 +18608,7 @@
       <c r="L78" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M78" s="433" t="s">
+      <c r="M78" s="408" t="s">
         <v>278</v>
       </c>
     </row>
@@ -18612,7 +18619,7 @@
       <c r="C79" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D79" s="431" t="s">
+      <c r="D79" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E79" s="29">
@@ -18627,7 +18634,7 @@
       <c r="L79" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M79" s="433" t="s">
+      <c r="M79" s="408" t="s">
         <v>279</v>
       </c>
     </row>
@@ -18638,7 +18645,7 @@
       <c r="C80" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D80" s="431" t="s">
+      <c r="D80" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E80" s="29">
@@ -18653,7 +18660,7 @@
       <c r="L80" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M80" s="433" t="s">
+      <c r="M80" s="408" t="s">
         <v>280</v>
       </c>
     </row>
@@ -18664,7 +18671,7 @@
       <c r="C81" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D81" s="431" t="s">
+      <c r="D81" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E81" s="29">
@@ -18679,7 +18686,7 @@
       <c r="L81" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M81" s="433" t="s">
+      <c r="M81" s="408" t="s">
         <v>281</v>
       </c>
     </row>
@@ -18690,7 +18697,7 @@
       <c r="C82" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D82" s="431" t="s">
+      <c r="D82" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E82" s="29">
@@ -18705,7 +18712,7 @@
       <c r="L82" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M82" s="433" t="s">
+      <c r="M82" s="408" t="s">
         <v>282</v>
       </c>
     </row>
@@ -18716,7 +18723,7 @@
       <c r="C83" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D83" s="431" t="s">
+      <c r="D83" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E83" s="29">
@@ -18731,7 +18738,7 @@
       <c r="L83" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M83" s="433" t="s">
+      <c r="M83" s="408" t="s">
         <v>283</v>
       </c>
     </row>
@@ -18742,7 +18749,7 @@
       <c r="C84" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D84" s="431" t="s">
+      <c r="D84" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E84" s="29">
@@ -18757,7 +18764,7 @@
       <c r="L84" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M84" s="433" t="s">
+      <c r="M84" s="408" t="s">
         <v>284</v>
       </c>
     </row>
@@ -18768,7 +18775,7 @@
       <c r="C85" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D85" s="431" t="s">
+      <c r="D85" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E85" s="29">
@@ -18783,7 +18790,7 @@
       <c r="L85" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M85" s="433" t="s">
+      <c r="M85" s="408" t="s">
         <v>285</v>
       </c>
     </row>
@@ -18794,7 +18801,7 @@
       <c r="C86" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D86" s="431" t="s">
+      <c r="D86" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E86" s="29">
@@ -18809,7 +18816,7 @@
       <c r="L86" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M86" s="433" t="s">
+      <c r="M86" s="408" t="s">
         <v>286</v>
       </c>
     </row>
@@ -18820,7 +18827,7 @@
       <c r="C87" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D87" s="431" t="s">
+      <c r="D87" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E87" s="29">
@@ -18835,7 +18842,7 @@
       <c r="L87" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M87" s="433" t="s">
+      <c r="M87" s="408" t="s">
         <v>287</v>
       </c>
     </row>
@@ -18846,7 +18853,7 @@
       <c r="C88" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="431" t="s">
+      <c r="D88" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E88" s="29">
@@ -18861,7 +18868,7 @@
       <c r="L88" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M88" s="433" t="s">
+      <c r="M88" s="408" t="s">
         <v>288</v>
       </c>
     </row>
@@ -18887,7 +18894,7 @@
       <c r="L89" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="M89" s="432" t="s">
+      <c r="M89" s="407" t="s">
         <v>289</v>
       </c>
     </row>
@@ -18898,7 +18905,7 @@
       <c r="C90" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D90" s="431" t="s">
+      <c r="D90" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E90" s="29">
@@ -18928,7 +18935,7 @@
       <c r="C91" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D91" s="431" t="s">
+      <c r="D91" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E91" s="29">
@@ -18961,7 +18968,7 @@
       <c r="C92" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D92" s="431" t="s">
+      <c r="D92" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E92" s="29">
@@ -18997,7 +19004,7 @@
       <c r="C93" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D93" s="431" t="s">
+      <c r="D93" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E93" s="29">
@@ -19030,7 +19037,7 @@
       <c r="C94" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D94" s="431" t="s">
+      <c r="D94" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E94" s="29">
@@ -19063,7 +19070,7 @@
       <c r="C95" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D95" s="431" t="s">
+      <c r="D95" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E95" s="29">
@@ -19096,7 +19103,7 @@
       <c r="C96" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D96" s="431" t="s">
+      <c r="D96" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E96" s="29">
@@ -19111,7 +19118,7 @@
       <c r="L96" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M96" s="433" t="s">
+      <c r="M96" s="408" t="s">
         <v>276</v>
       </c>
     </row>
@@ -19122,7 +19129,7 @@
       <c r="C97" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D97" s="431" t="s">
+      <c r="D97" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E97" s="29">
@@ -19137,7 +19144,7 @@
       <c r="L97" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M97" s="433" t="s">
+      <c r="M97" s="408" t="s">
         <v>277</v>
       </c>
     </row>
@@ -19148,7 +19155,7 @@
       <c r="C98" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D98" s="431" t="s">
+      <c r="D98" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E98" s="29">
@@ -19163,7 +19170,7 @@
       <c r="L98" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M98" s="433" t="s">
+      <c r="M98" s="408" t="s">
         <v>278</v>
       </c>
     </row>
@@ -19174,7 +19181,7 @@
       <c r="C99" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D99" s="431" t="s">
+      <c r="D99" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E99" s="29">
@@ -19189,7 +19196,7 @@
       <c r="L99" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M99" s="433" t="s">
+      <c r="M99" s="408" t="s">
         <v>279</v>
       </c>
     </row>
@@ -19200,7 +19207,7 @@
       <c r="C100" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D100" s="431" t="s">
+      <c r="D100" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E100" s="29">
@@ -19215,7 +19222,7 @@
       <c r="L100" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M100" s="433" t="s">
+      <c r="M100" s="408" t="s">
         <v>280</v>
       </c>
     </row>
@@ -19226,7 +19233,7 @@
       <c r="C101" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D101" s="431" t="s">
+      <c r="D101" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E101" s="29">
@@ -19241,7 +19248,7 @@
       <c r="L101" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M101" s="433" t="s">
+      <c r="M101" s="408" t="s">
         <v>281</v>
       </c>
     </row>
@@ -19252,7 +19259,7 @@
       <c r="C102" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D102" s="431" t="s">
+      <c r="D102" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E102" s="29">
@@ -19267,7 +19274,7 @@
       <c r="L102" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M102" s="433" t="s">
+      <c r="M102" s="408" t="s">
         <v>282</v>
       </c>
     </row>
@@ -19278,7 +19285,7 @@
       <c r="C103" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D103" s="431" t="s">
+      <c r="D103" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E103" s="29">
@@ -19293,7 +19300,7 @@
       <c r="L103" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M103" s="433" t="s">
+      <c r="M103" s="408" t="s">
         <v>283</v>
       </c>
     </row>
@@ -19304,7 +19311,7 @@
       <c r="C104" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D104" s="431" t="s">
+      <c r="D104" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E104" s="29">
@@ -19319,7 +19326,7 @@
       <c r="L104" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M104" s="433" t="s">
+      <c r="M104" s="408" t="s">
         <v>284</v>
       </c>
     </row>
@@ -19330,7 +19337,7 @@
       <c r="C105" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D105" s="431" t="s">
+      <c r="D105" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E105" s="29">
@@ -19345,7 +19352,7 @@
       <c r="L105" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M105" s="433" t="s">
+      <c r="M105" s="408" t="s">
         <v>285</v>
       </c>
     </row>
@@ -19356,7 +19363,7 @@
       <c r="C106" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D106" s="431" t="s">
+      <c r="D106" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E106" s="29">
@@ -19371,7 +19378,7 @@
       <c r="L106" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M106" s="433" t="s">
+      <c r="M106" s="408" t="s">
         <v>286</v>
       </c>
     </row>
@@ -19382,7 +19389,7 @@
       <c r="C107" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D107" s="431" t="s">
+      <c r="D107" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E107" s="29">
@@ -19397,7 +19404,7 @@
       <c r="L107" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M107" s="433" t="s">
+      <c r="M107" s="408" t="s">
         <v>287</v>
       </c>
     </row>
@@ -19408,7 +19415,7 @@
       <c r="C108" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D108" s="431" t="s">
+      <c r="D108" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E108" s="29">
@@ -19423,7 +19430,7 @@
       <c r="L108" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M108" s="433" t="s">
+      <c r="M108" s="408" t="s">
         <v>288</v>
       </c>
     </row>
@@ -19449,7 +19456,7 @@
       <c r="L109" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="M109" s="432" t="s">
+      <c r="M109" s="407" t="s">
         <v>289</v>
       </c>
     </row>
@@ -19460,7 +19467,7 @@
       <c r="C110" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D110" s="431" t="s">
+      <c r="D110" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E110" s="29">
@@ -19491,7 +19498,7 @@
       <c r="C111" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D111" s="431" t="s">
+      <c r="D111" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E111" s="29">
@@ -19520,7 +19527,7 @@
       <c r="C112" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D112" s="431" t="s">
+      <c r="D112" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E112" s="29">
@@ -19551,7 +19558,7 @@
       <c r="C113" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D113" s="431" t="s">
+      <c r="D113" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E113" s="29">
@@ -19582,7 +19589,7 @@
       <c r="C114" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D114" s="431" t="s">
+      <c r="D114" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E114" s="29">
@@ -19613,7 +19620,7 @@
       <c r="C115" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D115" s="431" t="s">
+      <c r="D115" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E115" s="29">
@@ -19644,7 +19651,7 @@
       <c r="C116" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D116" s="431" t="s">
+      <c r="D116" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E116" s="29">
@@ -19659,7 +19666,7 @@
       <c r="L116" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M116" s="433" t="s">
+      <c r="M116" s="408" t="s">
         <v>276</v>
       </c>
     </row>
@@ -19670,7 +19677,7 @@
       <c r="C117" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D117" s="431" t="s">
+      <c r="D117" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E117" s="29">
@@ -19685,7 +19692,7 @@
       <c r="L117" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M117" s="433" t="s">
+      <c r="M117" s="408" t="s">
         <v>277</v>
       </c>
     </row>
@@ -19696,7 +19703,7 @@
       <c r="C118" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D118" s="431" t="s">
+      <c r="D118" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E118" s="29">
@@ -19711,7 +19718,7 @@
       <c r="L118" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M118" s="433" t="s">
+      <c r="M118" s="408" t="s">
         <v>278</v>
       </c>
     </row>
@@ -19722,7 +19729,7 @@
       <c r="C119" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D119" s="431" t="s">
+      <c r="D119" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E119" s="29">
@@ -19737,7 +19744,7 @@
       <c r="L119" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M119" s="433" t="s">
+      <c r="M119" s="408" t="s">
         <v>279</v>
       </c>
     </row>
@@ -19748,7 +19755,7 @@
       <c r="C120" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D120" s="431" t="s">
+      <c r="D120" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E120" s="29">
@@ -19763,7 +19770,7 @@
       <c r="L120" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M120" s="433" t="s">
+      <c r="M120" s="408" t="s">
         <v>280</v>
       </c>
     </row>
@@ -19774,7 +19781,7 @@
       <c r="C121" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D121" s="431" t="s">
+      <c r="D121" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E121" s="29">
@@ -19789,7 +19796,7 @@
       <c r="L121" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M121" s="433" t="s">
+      <c r="M121" s="408" t="s">
         <v>281</v>
       </c>
     </row>
@@ -19800,7 +19807,7 @@
       <c r="C122" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D122" s="431" t="s">
+      <c r="D122" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E122" s="29">
@@ -19815,7 +19822,7 @@
       <c r="L122" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M122" s="433" t="s">
+      <c r="M122" s="408" t="s">
         <v>282</v>
       </c>
     </row>
@@ -19826,7 +19833,7 @@
       <c r="C123" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D123" s="431" t="s">
+      <c r="D123" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E123" s="29">
@@ -19841,7 +19848,7 @@
       <c r="L123" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M123" s="433" t="s">
+      <c r="M123" s="408" t="s">
         <v>283</v>
       </c>
     </row>
@@ -19852,7 +19859,7 @@
       <c r="C124" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D124" s="431" t="s">
+      <c r="D124" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E124" s="29">
@@ -19867,7 +19874,7 @@
       <c r="L124" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M124" s="433" t="s">
+      <c r="M124" s="408" t="s">
         <v>284</v>
       </c>
     </row>
@@ -19878,7 +19885,7 @@
       <c r="C125" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D125" s="431" t="s">
+      <c r="D125" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E125" s="29">
@@ -19893,7 +19900,7 @@
       <c r="L125" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M125" s="433" t="s">
+      <c r="M125" s="408" t="s">
         <v>285</v>
       </c>
     </row>
@@ -19904,7 +19911,7 @@
       <c r="C126" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D126" s="431" t="s">
+      <c r="D126" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E126" s="29">
@@ -19919,7 +19926,7 @@
       <c r="L126" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M126" s="433" t="s">
+      <c r="M126" s="408" t="s">
         <v>286</v>
       </c>
     </row>
@@ -19930,7 +19937,7 @@
       <c r="C127" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D127" s="431" t="s">
+      <c r="D127" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E127" s="29">
@@ -19945,7 +19952,7 @@
       <c r="L127" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M127" s="433" t="s">
+      <c r="M127" s="408" t="s">
         <v>287</v>
       </c>
     </row>
@@ -19956,7 +19963,7 @@
       <c r="C128" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D128" s="431" t="s">
+      <c r="D128" s="406" t="s">
         <v>264</v>
       </c>
       <c r="E128" s="29">
@@ -19971,7 +19978,7 @@
       <c r="L128" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M128" s="433" t="s">
+      <c r="M128" s="408" t="s">
         <v>288</v>
       </c>
     </row>
@@ -19999,7 +20006,7 @@
       <c r="L129" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="M129" s="432" t="s">
+      <c r="M129" s="407" t="s">
         <v>289</v>
       </c>
     </row>
@@ -20220,53 +20227,53 @@
         <f>AVA!$D$9</f>
         <v>IMPELC-DKNO</v>
       </c>
-      <c r="M10" s="404" t="s">
+      <c r="M10" s="413" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="408">
+      <c r="N10" s="417">
         <v>2010</v>
       </c>
-      <c r="O10" s="409"/>
-      <c r="P10" s="410" t="s">
+      <c r="O10" s="418"/>
+      <c r="P10" s="419" t="s">
         <v>31</v>
       </c>
-      <c r="Q10" s="411"/>
-      <c r="R10" s="410">
+      <c r="Q10" s="420"/>
+      <c r="R10" s="419">
         <v>2015</v>
       </c>
-      <c r="S10" s="411"/>
-      <c r="T10" s="410">
+      <c r="S10" s="420"/>
+      <c r="T10" s="419">
         <v>2016</v>
       </c>
-      <c r="U10" s="411"/>
-      <c r="V10" s="410">
+      <c r="U10" s="420"/>
+      <c r="V10" s="419">
         <v>2017</v>
       </c>
-      <c r="W10" s="411"/>
-      <c r="X10" s="410">
+      <c r="W10" s="420"/>
+      <c r="X10" s="419">
         <v>2018</v>
       </c>
-      <c r="Y10" s="411"/>
-      <c r="Z10" s="410">
+      <c r="Y10" s="420"/>
+      <c r="Z10" s="419">
         <v>2019</v>
       </c>
-      <c r="AA10" s="411"/>
-      <c r="AB10" s="410">
+      <c r="AA10" s="420"/>
+      <c r="AB10" s="419">
         <v>2020</v>
       </c>
-      <c r="AC10" s="411"/>
-      <c r="AD10" s="406">
+      <c r="AC10" s="420"/>
+      <c r="AD10" s="415">
         <v>2025</v>
       </c>
-      <c r="AE10" s="407"/>
-      <c r="AF10" s="406">
+      <c r="AE10" s="416"/>
+      <c r="AF10" s="415">
         <v>2030</v>
       </c>
-      <c r="AG10" s="407"/>
-      <c r="AH10" s="406">
+      <c r="AG10" s="416"/>
+      <c r="AH10" s="415">
         <v>2035</v>
       </c>
-      <c r="AI10" s="407"/>
+      <c r="AI10" s="416"/>
       <c r="AP10"/>
       <c r="AQ10"/>
       <c r="AR10"/>
@@ -20295,7 +20302,7 @@
         <f>AVA!$D$10</f>
         <v>EXPELC-DKNO</v>
       </c>
-      <c r="M11" s="405"/>
+      <c r="M11" s="414"/>
       <c r="N11" s="77" t="s">
         <v>14</v>
       </c>
@@ -22934,22 +22941,22 @@
       <c r="B7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="414">
+      <c r="C7" s="423">
         <v>2010</v>
       </c>
-      <c r="D7" s="415"/>
-      <c r="E7" s="414" t="s">
+      <c r="D7" s="424"/>
+      <c r="E7" s="423" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="415"/>
-      <c r="G7" s="414">
+      <c r="F7" s="424"/>
+      <c r="G7" s="423">
         <v>2014</v>
       </c>
-      <c r="H7" s="416"/>
-      <c r="I7" s="412" t="s">
+      <c r="H7" s="425"/>
+      <c r="I7" s="421" t="s">
         <v>215</v>
       </c>
-      <c r="J7" s="413"/>
+      <c r="J7" s="422"/>
       <c r="K7" s="346">
         <v>2018</v>
       </c>
@@ -22959,18 +22966,18 @@
         <v>2019</v>
       </c>
       <c r="N7" s="346"/>
-      <c r="O7" s="412" t="s">
+      <c r="O7" s="421" t="s">
         <v>221</v>
       </c>
-      <c r="P7" s="413"/>
+      <c r="P7" s="422"/>
       <c r="Q7" s="346">
         <v>2021</v>
       </c>
       <c r="R7" s="346"/>
-      <c r="S7" s="412" t="s">
+      <c r="S7" s="421" t="s">
         <v>222</v>
       </c>
-      <c r="T7" s="413"/>
+      <c r="T7" s="422"/>
       <c r="U7" s="352">
         <f>Udlandsforbindelser!X3</f>
         <v>2030</v>
@@ -28240,58 +28247,58 @@
       <c r="A3" s="158" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="420">
+      <c r="B3" s="429">
         <v>2015</v>
       </c>
-      <c r="C3" s="421"/>
-      <c r="D3" s="420">
+      <c r="C3" s="430"/>
+      <c r="D3" s="429">
         <v>2016</v>
       </c>
-      <c r="E3" s="421"/>
-      <c r="F3" s="419">
+      <c r="E3" s="430"/>
+      <c r="F3" s="428">
         <v>2017</v>
       </c>
-      <c r="G3" s="419"/>
-      <c r="H3" s="419">
+      <c r="G3" s="428"/>
+      <c r="H3" s="428">
         <v>2018</v>
       </c>
-      <c r="I3" s="420"/>
-      <c r="J3" s="419">
+      <c r="I3" s="429"/>
+      <c r="J3" s="428">
         <v>2019</v>
       </c>
-      <c r="K3" s="419"/>
-      <c r="L3" s="419">
+      <c r="K3" s="428"/>
+      <c r="L3" s="428">
         <v>2020</v>
       </c>
-      <c r="M3" s="420"/>
-      <c r="N3" s="419">
+      <c r="M3" s="429"/>
+      <c r="N3" s="428">
         <v>2021</v>
       </c>
-      <c r="O3" s="420"/>
-      <c r="P3" s="420">
+      <c r="O3" s="429"/>
+      <c r="P3" s="429">
         <v>2022</v>
       </c>
-      <c r="Q3" s="421"/>
-      <c r="R3" s="420">
+      <c r="Q3" s="430"/>
+      <c r="R3" s="429">
         <v>2023</v>
       </c>
-      <c r="S3" s="421"/>
-      <c r="T3" s="420">
+      <c r="S3" s="430"/>
+      <c r="T3" s="429">
         <v>2024</v>
       </c>
-      <c r="U3" s="421"/>
-      <c r="V3" s="417">
+      <c r="U3" s="430"/>
+      <c r="V3" s="426">
         <v>2025</v>
       </c>
-      <c r="W3" s="418"/>
-      <c r="X3" s="417">
+      <c r="W3" s="427"/>
+      <c r="X3" s="426">
         <v>2030</v>
       </c>
-      <c r="Y3" s="418"/>
-      <c r="Z3" s="422">
+      <c r="Y3" s="427"/>
+      <c r="Z3" s="431">
         <v>2035</v>
       </c>
-      <c r="AA3" s="417"/>
+      <c r="AA3" s="426"/>
     </row>
     <row r="4" spans="1:27">
       <c r="A4" s="157"/>
@@ -29470,13 +29477,13 @@
     </row>
     <row r="5" spans="2:8" ht="13.15" thickBot="1"/>
     <row r="6" spans="2:8" ht="25.9" customHeight="1">
-      <c r="B6" s="423" t="s">
+      <c r="B6" s="432" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="423" t="s">
+      <c r="C6" s="432" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="423" t="s">
+      <c r="D6" s="432" t="s">
         <v>78</v>
       </c>
       <c r="E6" s="114" t="s">
@@ -29485,25 +29492,25 @@
       <c r="F6" s="114" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="425" t="s">
+      <c r="G6" s="434" t="s">
         <v>82</v>
       </c>
-      <c r="H6" s="427" t="s">
+      <c r="H6" s="436" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="13.15" thickBot="1">
-      <c r="B7" s="424"/>
-      <c r="C7" s="424"/>
-      <c r="D7" s="424"/>
+      <c r="B7" s="433"/>
+      <c r="C7" s="433"/>
+      <c r="D7" s="433"/>
       <c r="E7" s="115" t="s">
         <v>80</v>
       </c>
       <c r="F7" s="115" t="s">
         <v>80</v>
       </c>
-      <c r="G7" s="426"/>
-      <c r="H7" s="428"/>
+      <c r="G7" s="435"/>
+      <c r="H7" s="437"/>
     </row>
     <row r="8" spans="2:8" ht="13.5" thickBot="1">
       <c r="B8" s="116" t="s">

</xml_diff>